<commit_message>
MAJ Simulateur Impôt - suppression des liaisons
</commit_message>
<xml_diff>
--- a/Simulateur Impôt 2025.xlsx
+++ b/Simulateur Impôt 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://15041946-my.sharepoint.com/personal/guillaume_guilbert_ext_plasticomnium_com/Documents/Documents/000-Perso/Conseil patrimoine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C0528B22-4170-4882-BFF7-495ED349E4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8EB4541-5F18-40D0-9D82-80623AF6D972}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{C0528B22-4170-4882-BFF7-495ED349E4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD9327CE-AB7F-4CA6-BE02-A86B68AB9EA8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F929243B-59AF-4C27-884B-2E1D5A5CA125}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{F929243B-59AF-4C27-884B-2E1D5A5CA125}"/>
   </bookViews>
   <sheets>
     <sheet name="MAJ" sheetId="3" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="Simulateur impôt 2025" sheetId="2" r:id="rId3"/>
     <sheet name="Simulateur impôt simplifié 2025" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1683,66 +1680,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="MAJ"/>
-      <sheetName val="Données"/>
-      <sheetName val="Simulateur impôt 2025"/>
-      <sheetName val="Simulateur impôt simplifié 2025"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="A3">
-            <v>0</v>
-          </cell>
-          <cell r="B3">
-            <v>11497</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>11497</v>
-          </cell>
-          <cell r="B4">
-            <v>29315</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>29315</v>
-          </cell>
-          <cell r="B5">
-            <v>83823</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>83823</v>
-          </cell>
-          <cell r="B6">
-            <v>180294</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>180294</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
@@ -2042,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E471562-FD17-47C0-9DA1-A1E9FE2F79C2}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2743,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBD7E57-C752-47CA-9FA3-2AC6F5061571}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,8 +2695,8 @@
     <col min="7" max="7" width="51.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="11" width="47.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2984,7 +2921,7 @@
         <v>121</v>
       </c>
       <c r="K13" s="93">
-        <f>IF(IF($H$11&gt;[1]Données!B3,[1]Données!B3,$H$11-[1]Données!A3)&lt;0,0,IF($H$11&gt;[1]Données!B3,[1]Données!B3,$H$11-[1]Données!A3))</f>
+        <f>IF(IF($H$11&gt;Données!B3,Données!B3,$H$11-Données!A3)&lt;0,0,IF($H$11&gt;Données!B3,Données!B3,$H$11-Données!A3))</f>
         <v>0</v>
       </c>
     </row>
@@ -3012,7 +2949,7 @@
         <v>122</v>
       </c>
       <c r="K14" s="93">
-        <f>IF(IF($H$11&gt;[1]Données!B4,[1]Données!B4,$H$11-[1]Données!A4)&lt;0,0,IF($H$11&gt;[1]Données!B4,[1]Données!B4,$H$11-[1]Données!A4))</f>
+        <f>IF(IF($H$11&gt;Données!B4,Données!B4,$H$11-Données!A4)&lt;0,0,IF($H$11&gt;Données!B4,Données!B4,$H$11-Données!A4))</f>
         <v>0</v>
       </c>
     </row>
@@ -3041,7 +2978,7 @@
         <v>123</v>
       </c>
       <c r="K15" s="93">
-        <f>IF(IF($H$11&gt;[1]Données!B5,[1]Données!B5,$H$11-[1]Données!A5)&lt;0,0,IF($H$11&gt;[1]Données!B5,[1]Données!B5,$H$11-[1]Données!A5))</f>
+        <f>IF(IF($H$11&gt;Données!B5,Données!B5,$H$11-Données!A5)&lt;0,0,IF($H$11&gt;Données!B5,Données!B5,$H$11-Données!A5))</f>
         <v>0</v>
       </c>
     </row>
@@ -3060,7 +2997,7 @@
         <v>124</v>
       </c>
       <c r="K16" s="93">
-        <f>IF(IF($H$11&gt;[1]Données!B6,[1]Données!B6,$H$11-[1]Données!A6)&lt;0,0,IF($H$11&gt;[1]Données!B6,[1]Données!B6,$H$11-[1]Données!A6))</f>
+        <f>IF(IF($H$11&gt;Données!B6,Données!B6,$H$11-Données!A6)&lt;0,0,IF($H$11&gt;Données!B6,Données!B6,$H$11-Données!A6))</f>
         <v>0</v>
       </c>
     </row>
@@ -3084,7 +3021,7 @@
         <v>125</v>
       </c>
       <c r="K17" s="93">
-        <f>IF((H11-[1]Données!A7)&lt;0,0,H11-[1]Données!A7)</f>
+        <f>IF((H11-Données!A7)&lt;0,0,H11-Données!A7)</f>
         <v>0</v>
       </c>
     </row>
@@ -3298,7 +3235,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{61FF6B5B-76F5-47A6-B377-712765BBC03B}">
           <x14:formula1>
             <xm:f>Données!$A$10:$A$14</xm:f>

</xml_diff>